<commit_message>
change hurt of diagonal
</commit_message>
<xml_diff>
--- a/src/server/probabilities/1.xlsx
+++ b/src/server/probabilities/1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\actions_P\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\dars\TAs\AI2_TA\src\server\probabilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBEAFDA-12A7-4304-91EC-30C37E4E5503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBE57CD-8E55-4EF5-9FD0-E105EF1EE080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="normal" sheetId="1" r:id="rId1"/>
@@ -380,8 +380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:K10"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.265625" defaultRowHeight="24.4" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -1469,7 +1469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7498E32B-0646-4260-9476-60B3C1593708}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>

</xml_diff>